<commit_message>
finish guia de usuario
</commit_message>
<xml_diff>
--- a/experiment/nonconvex/MitsosBarton2006Ex312/Experimentos_Generador/MitsosBarton2006Ex312__C_Stationarygenerator_alpha_non_zero.xlsx
+++ b/experiment/nonconvex/MitsosBarton2006Ex312/Experimentos_Generador/MitsosBarton2006Ex312__C_Stationarygenerator_alpha_non_zero.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Leader_Expr</t>
   </si>
@@ -87,10 +87,10 @@
     <t>Gamma_value</t>
   </si>
   <si>
-    <t>-1 + 19.753935879690562y</t>
-  </si>
-  <si>
-    <t>64.18798840297886</t>
+    <t>-1 - 2.16787934748732y</t>
+  </si>
+  <si>
+    <t>-8.154001846708155</t>
   </si>
   <si>
     <t>J_0_L0_v</t>
@@ -99,16 +99,16 @@
     <t>0.23</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>8.100000000000001</t>
-  </si>
-  <si>
-    <t>-1 + 0.5899551335322607y</t>
-  </si>
-  <si>
-    <t>0.9468519406564604</t>
+    <t>-0.1</t>
+  </si>
+  <si>
+    <t>-1.6</t>
+  </si>
+  <si>
+    <t>-1 + 0.26195154640202667y</t>
+  </si>
+  <si>
+    <t>-0.13555989687331194</t>
   </si>
   <si>
     <t>J_0_LP_v</t>
@@ -117,7 +117,10 @@
     <t>0.58</t>
   </si>
   <si>
-    <t>6.7</t>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>9.3</t>
   </si>
   <si>
     <t>x</t>
@@ -135,16 +138,16 @@
     <t>vec_bf</t>
   </si>
   <si>
-    <t>-48.70957922977757</t>
+    <t>-43.47731964699112</t>
   </si>
   <si>
     <t>vec_BF</t>
   </si>
   <si>
-    <t>0.6262961186870797</t>
-  </si>
-  <si>
-    <t>-97.50964960469246</t>
+    <t>2.791119793746624</t>
+  </si>
+  <si>
+    <t>-114.01536647030993</t>
   </si>
   <si>
     <t>vec_alpha</t>
@@ -646,7 +649,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -664,18 +667,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -693,12 +696,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -716,17 +719,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -744,12 +747,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0.4100448664677393</v>
+        <v>0.7380484535979733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>